<commit_message>
modified:   excel_main.py 	modified:   sample.xlsx
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,42 +422,112 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n">
-        <v>42</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>列名1</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>列名2</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>列名3</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>列名4</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>列名5</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>列名6</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>列名7</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" t="n">
-        <v>3</v>
+      <c r="E2" t="n">
+        <v>1234</v>
       </c>
     </row>
     <row r="3">
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>这是第三行, 第二列</t>
-        </is>
+      <c r="E3" t="n">
+        <v>1235</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" t="n">
-        <v>3</v>
+      <c r="E4" t="n">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>列名1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>列名2</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>列名3</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>列名4</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>列名5</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>列名6</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>列名7</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="E8" t="n">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="E9" t="n">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="E10" t="n">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="E11" t="n">
+        <v>1037</v>
       </c>
     </row>
   </sheetData>

</xml_diff>